<commit_message>
Done: Archieve mechanism with results
</commit_message>
<xml_diff>
--- a/src/classification_results.xlsx
+++ b/src/classification_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X8382\Documents\LTCIndexing\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B6C030-491F-477B-9749-4EFFD9C25A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAA5E84-F8D5-40A6-B5F7-080912A03D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Serial No</t>
   </si>
@@ -32,78 +32,6 @@
   </si>
   <si>
     <t>Classification</t>
-  </si>
-  <si>
-    <t>190150086 Complaint.TIF</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:48:59</t>
-  </si>
-  <si>
-    <t>Compliance</t>
-  </si>
-  <si>
-    <t>190169337 Complaint.tif</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:49:08</t>
-  </si>
-  <si>
-    <t>190224126 Appeal.TIF</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:49:42</t>
-  </si>
-  <si>
-    <t>190927373 Complaint doc.TIF</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:49:45</t>
-  </si>
-  <si>
-    <t>190994597 Complaint doc.TIF</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:49:48</t>
-  </si>
-  <si>
-    <t>190995424 Appeal.TIF</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:49:59</t>
-  </si>
-  <si>
-    <t>191009482 Complaint doc.tif</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:50:02</t>
-  </si>
-  <si>
-    <t>191031728 Appeal.TIF</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:51:00</t>
-  </si>
-  <si>
-    <t>191031795 Complaint doc.tif</t>
-  </si>
-  <si>
-    <t>2024-10-30 10:51:03</t>
-  </si>
-  <si>
-    <t>2024-10-30 11:17:38</t>
-  </si>
-  <si>
-    <t>2024-10-30 11:17:48</t>
-  </si>
-  <si>
-    <t>2024-10-30 11:18:26</t>
-  </si>
-  <si>
-    <t>2024-10-30 11:18:29</t>
-  </si>
-  <si>
-    <t>2024-10-30 11:18:33</t>
   </si>
 </sst>
 </file>
@@ -476,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,200 +433,376 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>5</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>